<commit_message>
DPCD and EDID information updated
spreadsheet describing contents of DisplayPort Configuration Data and
Extended Display Identification Data
</commit_message>
<xml_diff>
--- a/Documentation/DPCD.xlsx
+++ b/Documentation/DPCD.xlsx
@@ -13,8 +13,11 @@
   </bookViews>
   <sheets>
     <sheet name="DPCD" sheetId="2" r:id="rId1"/>
-    <sheet name="EDID" sheetId="3" r:id="rId2"/>
+    <sheet name="EDID" sheetId="5" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDID!#REF!</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="176">
   <si>
     <t>A</t>
   </si>
@@ -385,13 +388,184 @@
   </si>
   <si>
     <t>Automated Testing Sub-Field (optional)Z</t>
+  </si>
+  <si>
+    <t>Header</t>
+  </si>
+  <si>
+    <t>Manufacturer ID</t>
+  </si>
+  <si>
+    <t>Serial Number</t>
+  </si>
+  <si>
+    <t>Manufacture Date</t>
+  </si>
+  <si>
+    <t>EDID Version #</t>
+  </si>
+  <si>
+    <t>EDID Revision #</t>
+  </si>
+  <si>
+    <t>Video Input Type</t>
+  </si>
+  <si>
+    <t>Display Gamma</t>
+  </si>
+  <si>
+    <t>Supported Features</t>
+  </si>
+  <si>
+    <t>Color Characteristics</t>
+  </si>
+  <si>
+    <t>Manufacturers Reserved Timing</t>
+  </si>
+  <si>
+    <t>EDID Standard Timings Supported</t>
+  </si>
+  <si>
+    <t>Detailed Timing Descripter Block 1</t>
+  </si>
+  <si>
+    <t>Extension Flag</t>
+  </si>
+  <si>
+    <t>Checksum</t>
+  </si>
+  <si>
+    <t>Detailed Timing Descripter Block 2</t>
+  </si>
+  <si>
+    <t>Detailed Timing Descripter Block 3</t>
+  </si>
+  <si>
+    <t>Detailed Timing Descripter Block 4</t>
+  </si>
+  <si>
+    <t>A0</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>Product ID code</t>
+  </si>
+  <si>
+    <t>Horizontal Size</t>
+  </si>
+  <si>
+    <t>Vertical Size</t>
+  </si>
+  <si>
+    <t>Established Support Timings</t>
+  </si>
+  <si>
+    <t>Detailed Timing Descripter</t>
+  </si>
+  <si>
+    <t>FF</t>
+  </si>
+  <si>
+    <t>5A</t>
+  </si>
+  <si>
+    <t>1E</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>0E</t>
+  </si>
+  <si>
+    <t>2B</t>
+  </si>
+  <si>
+    <t>1B</t>
+  </si>
+  <si>
+    <t>2E</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>EF</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>0F</t>
+  </si>
+  <si>
+    <t>4F</t>
+  </si>
+  <si>
+    <t>1A</t>
+  </si>
+  <si>
+    <t>B0</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>1C</t>
+  </si>
+  <si>
+    <t>4E</t>
+  </si>
+  <si>
+    <t>0A</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>4B</t>
+  </si>
+  <si>
+    <t>FC</t>
+  </si>
+  <si>
+    <t>6D</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
+    <t>Hex</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>dec</t>
+  </si>
+  <si>
+    <t>Decription</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0#"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,8 +573,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -410,6 +590,54 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,7 +654,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -439,53 +667,90 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="6">
     <dxf>
       <fill>
         <patternFill>
@@ -525,174 +790,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4194,28 +4291,28 @@
     <mergeCell ref="E79:I79"/>
   </mergeCells>
   <conditionalFormatting sqref="A95:F101 E90:F93 E85:F88 E80:F83 E50:F78 E32:F48 E21:F30 E5:F19">
-    <cfRule type="expression" dxfId="11" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>NOT(EXACT($E5,$F5))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:H19 H21:H30 H32:H48 H50:H78 H80:H83 H85:H88 H90:H93 H95:H101">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"R/W"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"R"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:I19 I21:I30 I32:I48 I50:I78 I80:I83 I85:I88 I90:I93 I95:I101">
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="reserved">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="reserved">
       <formula>NOT(ISERROR(SEARCH("reserved",I5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E95:F101 E90:F93 E85:F88 E80:F83 E50:F78 E32:F48 E21:F30 E5:F19">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>EXACT($E5,$F5)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4225,12 +4322,3121 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="35"/>
+    <col min="2" max="2" width="4.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="7"/>
+    <col min="6" max="6" width="31.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="35" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="36">
+        <v>0</v>
+      </c>
+      <c r="B2" s="26">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="str">
+        <f>HEX2BIN(B2,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="D2" s="8">
+        <f>BIN2DEC(C2)</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="e">
+        <f>CHAR(D2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="36">
+        <f>A2+1</f>
+        <v>1</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="9" t="str">
+        <f t="shared" ref="C3:C66" si="0">HEX2BIN(B3,8)</f>
+        <v>11111111</v>
+      </c>
+      <c r="D3" s="8">
+        <f t="shared" ref="D3:D66" si="1">BIN2DEC(C3)</f>
+        <v>255</v>
+      </c>
+      <c r="E3" s="8" t="str">
+        <f t="shared" ref="E3:E66" si="2">CHAR(D3)</f>
+        <v>ÿ</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="36">
+        <f t="shared" ref="A4:A67" si="3">A3+1</f>
+        <v>2</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="D4" s="8">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="E4" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>ÿ</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="D5" s="8">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="E5" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>ÿ</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="36">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="D6" s="8">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="E6" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>ÿ</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="36">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="D7" s="8">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="E7" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>ÿ</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="36">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>11111111</v>
+      </c>
+      <c r="D8" s="8">
+        <f t="shared" si="1"/>
+        <v>255</v>
+      </c>
+      <c r="E8" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>ÿ</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="36">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="B9" s="26">
+        <v>0</v>
+      </c>
+      <c r="C9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="D9" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="37">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C10" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>01011010</v>
+      </c>
+      <c r="D10" s="10">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E10" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Z</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="37">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="B11" s="27">
+        <v>63</v>
+      </c>
+      <c r="C11" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>01100011</v>
+      </c>
+      <c r="D11" s="10">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+      <c r="E11" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>c</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="38">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="C12" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>00011110</v>
+      </c>
+      <c r="D12" s="12">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="E12" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001E_</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="38">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="C13" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>10101111</v>
+      </c>
+      <c r="D13" s="12">
+        <f t="shared" si="1"/>
+        <v>175</v>
+      </c>
+      <c r="E13" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>¯</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="39">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="B14" s="29">
+        <v>1</v>
+      </c>
+      <c r="C14" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="D14" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0001_</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="39">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="B15" s="29">
+        <v>1</v>
+      </c>
+      <c r="C15" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0001_</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="39">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="29">
+        <v>1</v>
+      </c>
+      <c r="C16" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E16" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0001_</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="39">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="B17" s="29">
+        <v>1</v>
+      </c>
+      <c r="C17" s="14" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="D17" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E17" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0001_</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="30">
+        <v>29</v>
+      </c>
+      <c r="C18" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>00101001</v>
+      </c>
+      <c r="D18" s="15">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="E18" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>)</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="40">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="30">
+        <v>11</v>
+      </c>
+      <c r="C19" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>00010001</v>
+      </c>
+      <c r="D19" s="15">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="E19" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0011_</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="41">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="31">
+        <v>1</v>
+      </c>
+      <c r="C20" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="D20" s="17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E20" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0001_</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="42">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="32">
+        <v>3</v>
+      </c>
+      <c r="C21" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>00000011</v>
+      </c>
+      <c r="D21" s="19">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E21" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0003_</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="43">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="22" t="str">
+        <f t="shared" si="0"/>
+        <v>00001110</v>
+      </c>
+      <c r="D22" s="21">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="E22" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x000E_</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="36">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="C23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>00101011</v>
+      </c>
+      <c r="D23" s="8">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="E23" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>+</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="37">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C24" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>00011011</v>
+      </c>
+      <c r="D24" s="10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="E24" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001B_</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="38">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="28">
+        <v>78</v>
+      </c>
+      <c r="C25" s="13" t="str">
+        <f t="shared" si="0"/>
+        <v>01111000</v>
+      </c>
+      <c r="D25" s="12">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+      <c r="E25" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>x</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="44">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>00101110</v>
+      </c>
+      <c r="D26" s="23">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="E26" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>.</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="40">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>11001111</v>
+      </c>
+      <c r="D27" s="15">
+        <f t="shared" si="1"/>
+        <v>207</v>
+      </c>
+      <c r="E27" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Ï</v>
+      </c>
+      <c r="F27" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="40">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>11000101</v>
+      </c>
+      <c r="D28" s="15">
+        <f t="shared" si="1"/>
+        <v>197</v>
+      </c>
+      <c r="E28" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Å</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="40">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="B29" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="C29" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>10100011</v>
+      </c>
+      <c r="D29" s="15">
+        <f t="shared" si="1"/>
+        <v>163</v>
+      </c>
+      <c r="E29" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>£</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="40">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="C30" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>01011010</v>
+      </c>
+      <c r="D30" s="15">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="E30" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Z</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="40">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="30">
+        <v>49</v>
+      </c>
+      <c r="C31" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>01001001</v>
+      </c>
+      <c r="D31" s="15">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+      <c r="E31" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>I</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="40">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C32" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>10100000</v>
+      </c>
+      <c r="D32" s="15">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="E32" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v> </v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="40">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="30">
+        <v>25</v>
+      </c>
+      <c r="C33" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>00100101</v>
+      </c>
+      <c r="D33" s="15">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="E33" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>%</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="40">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="30">
+        <v>12</v>
+      </c>
+      <c r="C34" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>00010010</v>
+      </c>
+      <c r="D34" s="15">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="E34" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0012_</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="40">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="B35" s="30">
+        <v>50</v>
+      </c>
+      <c r="C35" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>01010000</v>
+      </c>
+      <c r="D35" s="15">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+      <c r="E35" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>P</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="40">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="B36" s="30">
+        <v>54</v>
+      </c>
+      <c r="C36" s="16" t="str">
+        <f t="shared" si="0"/>
+        <v>01010100</v>
+      </c>
+      <c r="D36" s="15">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+      <c r="E36" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>T</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="41">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="B37" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="C37" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>10111111</v>
+      </c>
+      <c r="D37" s="17">
+        <f t="shared" si="1"/>
+        <v>191</v>
+      </c>
+      <c r="E37" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>¿</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="41">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="B38" s="31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="18" t="str">
+        <f t="shared" si="0"/>
+        <v>11101111</v>
+      </c>
+      <c r="D38" s="17">
+        <f t="shared" si="1"/>
+        <v>239</v>
+      </c>
+      <c r="E38" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>ï</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="42">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="B39" s="32">
+        <v>80</v>
+      </c>
+      <c r="C39" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>10000000</v>
+      </c>
+      <c r="D39" s="19">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="E39" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>€</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="43">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="B40" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="22" t="str">
+        <f>HEX2BIN(B40,8)</f>
+        <v>10110011</v>
+      </c>
+      <c r="D40" s="21">
+        <f>BIN2DEC(C40)</f>
+        <v>179</v>
+      </c>
+      <c r="E40" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>³</v>
+      </c>
+      <c r="F40" s="21" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="36">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="B41" s="26">
+        <v>0</v>
+      </c>
+      <c r="C41" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="D41" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="36">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="B42" s="26">
+        <v>95</v>
+      </c>
+      <c r="C42" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>10010101</v>
+      </c>
+      <c r="D42" s="8">
+        <f t="shared" si="1"/>
+        <v>149</v>
+      </c>
+      <c r="E42" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>•</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="36">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="B43" s="26">
+        <v>0</v>
+      </c>
+      <c r="C43" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>00000000</v>
+      </c>
+      <c r="D43" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="8" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="36">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="B44" s="26">
+        <v>95</v>
+      </c>
+      <c r="C44" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>10010101</v>
+      </c>
+      <c r="D44" s="8">
+        <f t="shared" si="1"/>
+        <v>149</v>
+      </c>
+      <c r="E44" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>•</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="36">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>158</v>
+      </c>
+      <c r="C45" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>00001111</v>
+      </c>
+      <c r="D45" s="8">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="E45" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x000F_</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="36">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="B46" s="26">
+        <v>90</v>
+      </c>
+      <c r="C46" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>10010000</v>
+      </c>
+      <c r="D46" s="8">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="E46" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v></v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="36">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="B47" s="26">
+        <v>40</v>
+      </c>
+      <c r="C47" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>01000000</v>
+      </c>
+      <c r="D47" s="8">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="E47" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>@</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="36">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="B48" s="26">
+        <v>81</v>
+      </c>
+      <c r="C48" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>10000001</v>
+      </c>
+      <c r="D48" s="8">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="E48" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v></v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="36">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="B49" s="26">
+        <v>80</v>
+      </c>
+      <c r="C49" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>10000000</v>
+      </c>
+      <c r="D49" s="8">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+      <c r="E49" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>€</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="36">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="B50" s="26">
+        <v>81</v>
+      </c>
+      <c r="C50" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>10000001</v>
+      </c>
+      <c r="D50" s="8">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+      <c r="E50" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v></v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="36">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="B51" s="26">
+        <v>40</v>
+      </c>
+      <c r="C51" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>01000000</v>
+      </c>
+      <c r="D51" s="8">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="E51" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>@</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="36">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="B52" s="26">
+        <v>71</v>
+      </c>
+      <c r="C52" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>01110001</v>
+      </c>
+      <c r="D52" s="8">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="E52" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>q</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="36">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>159</v>
+      </c>
+      <c r="C53" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>01001111</v>
+      </c>
+      <c r="D53" s="8">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+      <c r="E53" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>O</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="36">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="B54" s="26">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="D54" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E54" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0001_</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="36">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+      <c r="B55" s="26">
+        <v>1</v>
+      </c>
+      <c r="C55" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>00000001</v>
+      </c>
+      <c r="D55" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E55" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x0001_</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="37">
+        <f t="shared" si="3"/>
+        <v>54</v>
+      </c>
+      <c r="B56" s="27">
+        <v>21</v>
+      </c>
+      <c r="C56" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>00100001</v>
+      </c>
+      <c r="D56" s="10">
+        <f>BIN2DEC(C56)</f>
+        <v>33</v>
+      </c>
+      <c r="E56" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>!</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G56" t="str">
+        <f>CONCATENATE(B57,B56)</f>
+        <v>3921</v>
+      </c>
+      <c r="H56">
+        <f>HEX2DEC(G56)</f>
+        <v>14625</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="37">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="B57" s="27">
+        <v>39</v>
+      </c>
+      <c r="C57" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>00111001</v>
+      </c>
+      <c r="D57" s="10">
+        <f t="shared" si="1"/>
+        <v>57</v>
+      </c>
+      <c r="E57" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="F57" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="37">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+      <c r="B58" s="27">
+        <v>90</v>
+      </c>
+      <c r="C58" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>10010000</v>
+      </c>
+      <c r="D58" s="10">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="E58" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v></v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="37">
+        <f t="shared" si="3"/>
+        <v>57</v>
+      </c>
+      <c r="B59" s="27">
+        <v>30</v>
+      </c>
+      <c r="C59" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>00110000</v>
+      </c>
+      <c r="D59" s="10">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="E59" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="37">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+      <c r="B60" s="27">
+        <v>62</v>
+      </c>
+      <c r="C60" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>01100010</v>
+      </c>
+      <c r="D60" s="10">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+      <c r="E60" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>b</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="37">
+        <f t="shared" si="3"/>
+        <v>59</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="C61" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>00011010</v>
+      </c>
+      <c r="D61" s="10">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="E61" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>_x001A_</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="37">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+      <c r="B62" s="27">
+        <v>27</v>
+      </c>
+      <c r="C62" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>00100111</v>
+      </c>
+      <c r="D62" s="10">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="E62" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>'</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="37">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="B63" s="27">
+        <v>40</v>
+      </c>
+      <c r="C63" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>01000000</v>
+      </c>
+      <c r="D63" s="10">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="E63" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>@</v>
+      </c>
+      <c r="F63" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="37">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+      <c r="B64" s="27">
+        <v>68</v>
+      </c>
+      <c r="C64" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>01101000</v>
+      </c>
+      <c r="D64" s="10">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="E64" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>h</v>
+      </c>
+      <c r="F64" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="37">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+      <c r="B65" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>10110000</v>
+      </c>
+      <c r="D65" s="10">
+        <f t="shared" si="1"/>
+        <v>176</v>
+      </c>
+      <c r="E65" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>°</v>
+      </c>
+      <c r="F65" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="37">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="B66" s="27">
+        <v>36</v>
+      </c>
+      <c r="C66" s="11" t="str">
+        <f t="shared" si="0"/>
+        <v>00110110</v>
+      </c>
+      <c r="D66" s="10">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="E66" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="F66" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="37">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="B67" s="27">
+        <v>0</v>
+      </c>
+      <c r="C67" s="11" t="str">
+        <f t="shared" ref="C67:C129" si="4">HEX2BIN(B67,8)</f>
+        <v>00000000</v>
+      </c>
+      <c r="D67" s="10">
+        <f t="shared" ref="D67:D129" si="5">BIN2DEC(C67)</f>
+        <v>0</v>
+      </c>
+      <c r="E67" s="8" t="e">
+        <f t="shared" ref="E67:E129" si="6">CHAR(D67)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="37">
+        <f t="shared" ref="A68:A129" si="7">A67+1</f>
+        <v>66</v>
+      </c>
+      <c r="B68" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C68" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>10110001</v>
+      </c>
+      <c r="D68" s="10">
+        <f t="shared" si="5"/>
+        <v>177</v>
+      </c>
+      <c r="E68" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>±</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" s="37">
+        <f t="shared" si="7"/>
+        <v>67</v>
+      </c>
+      <c r="B69" s="27" t="s">
+        <v>158</v>
+      </c>
+      <c r="C69" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>00001111</v>
+      </c>
+      <c r="D69" s="10">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="E69" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>_x000F_</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" s="37">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+      <c r="B70" s="27">
+        <v>11</v>
+      </c>
+      <c r="C70" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>00010001</v>
+      </c>
+      <c r="D70" s="10">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="E70" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>_x0011_</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" s="37">
+        <f t="shared" si="7"/>
+        <v>69</v>
+      </c>
+      <c r="B71" s="27">
+        <v>0</v>
+      </c>
+      <c r="C71" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D71" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E71" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F71" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" s="37">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+      <c r="B72" s="27">
+        <v>0</v>
+      </c>
+      <c r="C72" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D72" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E72" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F72" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="38">
+        <f t="shared" si="7"/>
+        <v>71</v>
+      </c>
+      <c r="B73" s="28" t="s">
+        <v>163</v>
+      </c>
+      <c r="C73" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00011100</v>
+      </c>
+      <c r="D73" s="12">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="E73" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>_x001C_</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="38">
+        <f t="shared" si="7"/>
+        <v>72</v>
+      </c>
+      <c r="B74" s="28">
+        <v>0</v>
+      </c>
+      <c r="C74" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D74" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E74" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="38">
+        <f t="shared" si="7"/>
+        <v>73</v>
+      </c>
+      <c r="B75" s="28">
+        <v>0</v>
+      </c>
+      <c r="C75" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D75" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E75" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="38">
+        <f t="shared" si="7"/>
+        <v>74</v>
+      </c>
+      <c r="B76" s="28">
+        <v>0</v>
+      </c>
+      <c r="C76" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D76" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E76" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="38">
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+      <c r="B77" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="C77" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>11111111</v>
+      </c>
+      <c r="D77" s="12">
+        <f t="shared" si="5"/>
+        <v>255</v>
+      </c>
+      <c r="E77" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>ÿ</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="38">
+        <f t="shared" si="7"/>
+        <v>76</v>
+      </c>
+      <c r="B78" s="28">
+        <v>0</v>
+      </c>
+      <c r="C78" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D78" s="12">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E78" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="38">
+        <f t="shared" si="7"/>
+        <v>77</v>
+      </c>
+      <c r="B79" s="28">
+        <v>51</v>
+      </c>
+      <c r="C79" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>01010001</v>
+      </c>
+      <c r="D79" s="12">
+        <f t="shared" si="5"/>
+        <v>81</v>
+      </c>
+      <c r="E79" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>Q</v>
+      </c>
+      <c r="F79" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="38">
+        <f t="shared" si="7"/>
+        <v>78</v>
+      </c>
+      <c r="B80" s="28">
+        <v>43</v>
+      </c>
+      <c r="C80" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>01000011</v>
+      </c>
+      <c r="D80" s="12">
+        <f t="shared" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="E80" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>C</v>
+      </c>
+      <c r="F80" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="38">
+        <f t="shared" si="7"/>
+        <v>79</v>
+      </c>
+      <c r="B81" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="C81" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>01001110</v>
+      </c>
+      <c r="D81" s="12">
+        <f t="shared" si="5"/>
+        <v>78</v>
+      </c>
+      <c r="E81" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>N</v>
+      </c>
+      <c r="F81" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="38">
+        <f t="shared" si="7"/>
+        <v>80</v>
+      </c>
+      <c r="B82" s="28">
+        <v>30</v>
+      </c>
+      <c r="C82" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110000</v>
+      </c>
+      <c r="D82" s="12">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="E82" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F82" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="38">
+        <f t="shared" si="7"/>
+        <v>81</v>
+      </c>
+      <c r="B83" s="28">
+        <v>37</v>
+      </c>
+      <c r="C83" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110111</v>
+      </c>
+      <c r="D83" s="12">
+        <f t="shared" si="5"/>
+        <v>55</v>
+      </c>
+      <c r="E83" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>7</v>
+      </c>
+      <c r="F83" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="38">
+        <f t="shared" si="7"/>
+        <v>82</v>
+      </c>
+      <c r="B84" s="28">
+        <v>34</v>
+      </c>
+      <c r="C84" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110100</v>
+      </c>
+      <c r="D84" s="12">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="E84" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F84" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="38">
+        <f t="shared" si="7"/>
+        <v>83</v>
+      </c>
+      <c r="B85" s="28">
+        <v>31</v>
+      </c>
+      <c r="C85" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110001</v>
+      </c>
+      <c r="D85" s="12">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="E85" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F85" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="38">
+        <f t="shared" si="7"/>
+        <v>84</v>
+      </c>
+      <c r="B86" s="28">
+        <v>34</v>
+      </c>
+      <c r="C86" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110100</v>
+      </c>
+      <c r="D86" s="12">
+        <f t="shared" si="5"/>
+        <v>52</v>
+      </c>
+      <c r="E86" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="F86" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="38">
+        <f t="shared" si="7"/>
+        <v>85</v>
+      </c>
+      <c r="B87" s="28">
+        <v>30</v>
+      </c>
+      <c r="C87" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110000</v>
+      </c>
+      <c r="D87" s="12">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="E87" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F87" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="38">
+        <f t="shared" si="7"/>
+        <v>86</v>
+      </c>
+      <c r="B88" s="28">
+        <v>31</v>
+      </c>
+      <c r="C88" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110001</v>
+      </c>
+      <c r="D88" s="12">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="E88" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="F88" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="38">
+        <f t="shared" si="7"/>
+        <v>87</v>
+      </c>
+      <c r="B89" s="28">
+        <v>30</v>
+      </c>
+      <c r="C89" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110000</v>
+      </c>
+      <c r="D89" s="12">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="E89" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F89" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="38">
+        <f t="shared" si="7"/>
+        <v>88</v>
+      </c>
+      <c r="B90" s="28">
+        <v>32</v>
+      </c>
+      <c r="C90" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00110010</v>
+      </c>
+      <c r="D90" s="12">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="E90" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="F90" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="38">
+        <f t="shared" si="7"/>
+        <v>89</v>
+      </c>
+      <c r="B91" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="C91" s="13" t="str">
+        <f t="shared" si="4"/>
+        <v>00001010</v>
+      </c>
+      <c r="D91" s="12">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E91" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">
+</v>
+      </c>
+      <c r="F91" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="39">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="B92" s="29">
+        <v>0</v>
+      </c>
+      <c r="C92" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D92" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E92" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F92" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="39">
+        <f t="shared" si="7"/>
+        <v>91</v>
+      </c>
+      <c r="B93" s="29">
+        <v>0</v>
+      </c>
+      <c r="C93" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D93" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E93" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F93" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="39">
+        <f t="shared" si="7"/>
+        <v>92</v>
+      </c>
+      <c r="B94" s="29">
+        <v>0</v>
+      </c>
+      <c r="C94" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D94" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E94" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F94" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A95" s="39">
+        <f t="shared" si="7"/>
+        <v>93</v>
+      </c>
+      <c r="B95" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="C95" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>11111101</v>
+      </c>
+      <c r="D95" s="6">
+        <f t="shared" si="5"/>
+        <v>253</v>
+      </c>
+      <c r="E95" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>ý</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A96" s="39">
+        <f t="shared" si="7"/>
+        <v>94</v>
+      </c>
+      <c r="B96" s="29">
+        <v>0</v>
+      </c>
+      <c r="C96" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D96" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E96" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F96" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A97" s="39">
+        <f t="shared" si="7"/>
+        <v>95</v>
+      </c>
+      <c r="B97" s="29">
+        <v>32</v>
+      </c>
+      <c r="C97" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00110010</v>
+      </c>
+      <c r="D97" s="6">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="E97" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" s="39">
+        <f t="shared" si="7"/>
+        <v>96</v>
+      </c>
+      <c r="B98" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="C98" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>01001011</v>
+      </c>
+      <c r="D98" s="6">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="E98" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>K</v>
+      </c>
+      <c r="F98" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" s="39">
+        <f t="shared" si="7"/>
+        <v>97</v>
+      </c>
+      <c r="B99" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C99" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00011110</v>
+      </c>
+      <c r="D99" s="6">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="E99" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>_x001E_</v>
+      </c>
+      <c r="F99" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="39">
+        <f t="shared" si="7"/>
+        <v>98</v>
+      </c>
+      <c r="B100" s="29">
+        <v>52</v>
+      </c>
+      <c r="C100" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>01010010</v>
+      </c>
+      <c r="D100" s="6">
+        <f t="shared" si="5"/>
+        <v>82</v>
+      </c>
+      <c r="E100" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>R</v>
+      </c>
+      <c r="F100" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" s="39">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="B101" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="C101" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00001111</v>
+      </c>
+      <c r="D101" s="6">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="E101" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>_x000F_</v>
+      </c>
+      <c r="F101" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A102" s="39">
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+      <c r="B102" s="29">
+        <v>0</v>
+      </c>
+      <c r="C102" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D102" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E102" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F102" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" s="39">
+        <f t="shared" si="7"/>
+        <v>101</v>
+      </c>
+      <c r="B103" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C103" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00001010</v>
+      </c>
+      <c r="D103" s="6">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E103" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">
+</v>
+      </c>
+      <c r="F103" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" s="39">
+        <f t="shared" si="7"/>
+        <v>102</v>
+      </c>
+      <c r="B104" s="29">
+        <v>20</v>
+      </c>
+      <c r="C104" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D104" s="6">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E104" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F104" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="39">
+        <f t="shared" si="7"/>
+        <v>103</v>
+      </c>
+      <c r="B105" s="29">
+        <v>20</v>
+      </c>
+      <c r="C105" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D105" s="6">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E105" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="39">
+        <f t="shared" si="7"/>
+        <v>104</v>
+      </c>
+      <c r="B106" s="29">
+        <v>20</v>
+      </c>
+      <c r="C106" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D106" s="6">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E106" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F106" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="39">
+        <f t="shared" si="7"/>
+        <v>105</v>
+      </c>
+      <c r="B107" s="29">
+        <v>20</v>
+      </c>
+      <c r="C107" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D107" s="6">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E107" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F107" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A108" s="39">
+        <f t="shared" si="7"/>
+        <v>106</v>
+      </c>
+      <c r="B108" s="29">
+        <v>20</v>
+      </c>
+      <c r="C108" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D108" s="6">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E108" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A109" s="39">
+        <f t="shared" si="7"/>
+        <v>107</v>
+      </c>
+      <c r="B109" s="29">
+        <v>20</v>
+      </c>
+      <c r="C109" s="14" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D109" s="6">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E109" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F109" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A110" s="40">
+        <f t="shared" si="7"/>
+        <v>108</v>
+      </c>
+      <c r="B110" s="30">
+        <v>0</v>
+      </c>
+      <c r="C110" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D110" s="15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E110" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F110" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A111" s="40">
+        <f t="shared" si="7"/>
+        <v>109</v>
+      </c>
+      <c r="B111" s="30">
+        <v>0</v>
+      </c>
+      <c r="C111" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D111" s="15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E111" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F111" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A112" s="40">
+        <f t="shared" si="7"/>
+        <v>110</v>
+      </c>
+      <c r="B112" s="30">
+        <v>0</v>
+      </c>
+      <c r="C112" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D112" s="15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E112" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F112" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="40">
+        <f t="shared" si="7"/>
+        <v>111</v>
+      </c>
+      <c r="B113" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="C113" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>11111100</v>
+      </c>
+      <c r="D113" s="15">
+        <f t="shared" si="5"/>
+        <v>252</v>
+      </c>
+      <c r="E113" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>ü</v>
+      </c>
+      <c r="F113" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="40">
+        <f t="shared" si="7"/>
+        <v>112</v>
+      </c>
+      <c r="B114" s="30">
+        <v>0</v>
+      </c>
+      <c r="C114" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D114" s="15">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E114" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F114" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="40">
+        <f t="shared" si="7"/>
+        <v>113</v>
+      </c>
+      <c r="B115" s="30">
+        <v>56</v>
+      </c>
+      <c r="C115" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>01010110</v>
+      </c>
+      <c r="D115" s="15">
+        <f t="shared" si="5"/>
+        <v>86</v>
+      </c>
+      <c r="E115" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>V</v>
+      </c>
+      <c r="F115" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="40">
+        <f t="shared" si="7"/>
+        <v>114</v>
+      </c>
+      <c r="B116" s="30">
+        <v>58</v>
+      </c>
+      <c r="C116" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>01011000</v>
+      </c>
+      <c r="D116" s="15">
+        <f t="shared" si="5"/>
+        <v>88</v>
+      </c>
+      <c r="E116" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>X</v>
+      </c>
+      <c r="F116" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="40">
+        <f t="shared" si="7"/>
+        <v>115</v>
+      </c>
+      <c r="B117" s="30">
+        <v>32</v>
+      </c>
+      <c r="C117" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00110010</v>
+      </c>
+      <c r="D117" s="15">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="E117" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
+      <c r="F117" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="40">
+        <f t="shared" si="7"/>
+        <v>116</v>
+      </c>
+      <c r="B118" s="30">
+        <v>30</v>
+      </c>
+      <c r="C118" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00110000</v>
+      </c>
+      <c r="D118" s="15">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="E118" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F118" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" s="40">
+        <f t="shared" si="7"/>
+        <v>117</v>
+      </c>
+      <c r="B119" s="30">
+        <v>33</v>
+      </c>
+      <c r="C119" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00110011</v>
+      </c>
+      <c r="D119" s="15">
+        <f t="shared" si="5"/>
+        <v>51</v>
+      </c>
+      <c r="E119" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>3</v>
+      </c>
+      <c r="F119" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="40">
+        <f t="shared" si="7"/>
+        <v>118</v>
+      </c>
+      <c r="B120" s="30">
+        <v>35</v>
+      </c>
+      <c r="C120" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00110101</v>
+      </c>
+      <c r="D120" s="15">
+        <f t="shared" si="5"/>
+        <v>53</v>
+      </c>
+      <c r="E120" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>5</v>
+      </c>
+      <c r="F120" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="40">
+        <f t="shared" si="7"/>
+        <v>119</v>
+      </c>
+      <c r="B121" s="30">
+        <v>77</v>
+      </c>
+      <c r="C121" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>01110111</v>
+      </c>
+      <c r="D121" s="15">
+        <f t="shared" si="5"/>
+        <v>119</v>
+      </c>
+      <c r="E121" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>w</v>
+      </c>
+      <c r="F121" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="40">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+      <c r="B122" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="C122" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>01101101</v>
+      </c>
+      <c r="D122" s="15">
+        <f t="shared" si="5"/>
+        <v>109</v>
+      </c>
+      <c r="E122" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>m</v>
+      </c>
+      <c r="F122" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="40">
+        <f t="shared" si="7"/>
+        <v>121</v>
+      </c>
+      <c r="B123" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="C123" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00001010</v>
+      </c>
+      <c r="D123" s="15">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="E123" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve">
+</v>
+      </c>
+      <c r="F123" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="40">
+        <f t="shared" si="7"/>
+        <v>122</v>
+      </c>
+      <c r="B124" s="30">
+        <v>20</v>
+      </c>
+      <c r="C124" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D124" s="15">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E124" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F124" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="40">
+        <f t="shared" si="7"/>
+        <v>123</v>
+      </c>
+      <c r="B125" s="30">
+        <v>20</v>
+      </c>
+      <c r="C125" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D125" s="15">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E125" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F125" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="40">
+        <f t="shared" si="7"/>
+        <v>124</v>
+      </c>
+      <c r="B126" s="30">
+        <v>20</v>
+      </c>
+      <c r="C126" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D126" s="15">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E126" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F126" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="40">
+        <f t="shared" si="7"/>
+        <v>125</v>
+      </c>
+      <c r="B127" s="30">
+        <v>20</v>
+      </c>
+      <c r="C127" s="16" t="str">
+        <f t="shared" si="4"/>
+        <v>00100000</v>
+      </c>
+      <c r="D127" s="15">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="E127" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="F127" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="41">
+        <f t="shared" si="7"/>
+        <v>126</v>
+      </c>
+      <c r="B128" s="31">
+        <v>0</v>
+      </c>
+      <c r="C128" s="18" t="str">
+        <f t="shared" si="4"/>
+        <v>00000000</v>
+      </c>
+      <c r="D128" s="17">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E128" s="8" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F128" s="17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A129" s="42">
+        <f t="shared" si="7"/>
+        <v>127</v>
+      </c>
+      <c r="B129" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C129" s="20" t="str">
+        <f t="shared" si="4"/>
+        <v>11110010</v>
+      </c>
+      <c r="D129" s="19">
+        <f t="shared" si="5"/>
+        <v>242</v>
+      </c>
+      <c r="E129" s="8" t="str">
+        <f t="shared" si="6"/>
+        <v>ò</v>
+      </c>
+      <c r="F129" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>